<commit_message>
Get daily reddit data: Tue Jul 23 08:10:36 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_28.xlsx
+++ b/data/2024_07_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C478"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3015 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1ea2a0j</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>How long did you wear gel nails for the longest time?</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g5i4r3dy68ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1ea1pj1</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Fruit Nails!!!!</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ea1pj1</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1ea148y</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>doing my nails alone is a challenge but I love them 😍</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20k68qaat7ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1ea0bpg</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Lavender Haze</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ea0bpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1ea066x</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my fourth gel-x set done on myself </t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6bci3wai7ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1ea021p</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Random PSA! (For anyone who doesn’t know)</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ea021p/random_psa_for_anyone_who_doesnt_know/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1e9zzoh</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Worst nails :/</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9zzoh</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1e9zmfe</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new set! </t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9zmfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1e9zajy</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Long nails growth</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dw4ygzif87ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1e9z6zl</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Do fills make your acrylic weak?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7mxnjad77ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1e9z0ik</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gel on short natural nails </t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9z0ik</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1e9xdg0</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Birthday nails! I'm in love!</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9xdg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1e9xhz3</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Getting paint on natural nails after having acrylic?</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9xhz3/getting_paint_on_natural_nails_after_having/</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1e9ybxt</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Pastels 🥹💖</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmuk142ny6ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1e9y8x0</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>What do these options mean?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxds06ysx6ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1e9xwz0</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>I love them</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2yy24u1u6ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1e9xu4e</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Question for nail techs: are short nails annoying to work with?</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9xu4e/question_for_nail_techs_are_short_nails_annoying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1e9xr1m</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Galaxy press ons</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9xr1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1e9xq44</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>independent nail tech near kuta, bali?</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9xq44/independent_nail_tech_near_kuta_bali/</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1e9x8y5</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>can i get acrylics with my nails this short?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vskm7liao6ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1e9x257</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>HELP</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zv98egaim6ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1e9wi3t</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Really proud of my natural nails rn</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9wi3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1e9trv3</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Why does my top coat peel off after only 1 day?</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9trv3/why_does_my_top_coat_peel_off_after_only_1_day/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1e9wghp</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Cutie graduation nails</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n62havv6h6ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1e9wadq</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Dragon nails</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6qlw07qf6ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1e9w2y4</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Witch in black 🖤🌙</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9w2y4</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1e9w0zn</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>First time with acrylic nails since 2017</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9w0zn</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1e9w0i1</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Any sailor moon fans here? I love wearing art on my nails</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9w0i1</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1e9vqv5</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>This red in the sun is so 😍</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcdyjui4b6ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1e9vq31</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>1st time doung acrylics!</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bzqebxxa6ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1e9voce</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I want green… and glitter </t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9uzk50wja6ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1e9vm5v</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Coffin or Almond?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9vm5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1e9vemh</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>did my first set of gel nail tips with some designs :o</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4frdgwg886ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1e9ungs</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>New set ✨</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9ungs</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1e9u0tv</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Forgot to do an apex? Am I in trouble?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9u0tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1e9tzz7</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">There's something about green nails that makes me want to wear rings </t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yozw9c88w5ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1e9ttw8</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Pretty proud of these!</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v2qfw4iuu5ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1e9tnqt</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>First time trying polygel!</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4r8pu3gt5ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1e9sxqo</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Is this worth a $70 fill?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9sxqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1e9tj7u</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just broke my pinky soooo low. I’m getting married in 2 weeks. Are they gonna be able to put gel over this? </t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ztdlb8vgs5ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1e9sd1h</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>how do i remove gel x</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9sd1h/how_do_i_remove_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1e9sw2o</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Newbie help with press on nails!</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9sw2o/newbie_help_with_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1e9szuz</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What would you do if nail tech made you bleed? </t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9szuz/what_would_you_do_if_nail_tech_made_you_bleed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1e9tcsj</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Recommendations to get ‘natural’ look</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9tcsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1e9sp84</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Beetles Nail Glue vs ApresExtend Gel?</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9sp84/beetles_nail_glue_vs_apresextend_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1e9sjf8</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Did I over react?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9sjf8</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1e9s8xz</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you use different base gels for dip powder or should you stick to the one sold by the brand? </t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9s8xz/can_you_use_different_base_gels_for_dip_powder_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1e9s4bd</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>New set of acrylics. Loving the colour the nail tech suggested.</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5pe07vjdh5ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1e9rqgv</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8z357c4fe5ed1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1e9rn67</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Pink 🩷✨️✨️</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzw3l4nqd5ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1e9rfw4</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>We got the cutest nails</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3lplvn7c5ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1e9qz0g</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Decided to go with white  and i can say i don’t regret it </t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tllun7do85ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1e9qx27</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>What colour nails would you put with this dress?</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/598vdf5a85ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1e9qhhl</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How bad is it? Help </t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9qhhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1e9q6fo</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Aftercare tips?</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3tfjt3gt25ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1e9q2gh</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My gel nails ALWAYS chip </t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9q2gh/my_gel_nails_always_chip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1e9pzh3</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Baby boomers They like? 🩷</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cj7use3g15ed1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1e9pwfh</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Portland OR Nail Tech Recs?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9pwfh/portland_or_nail_tech_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1e9pmh5</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Mermaid set on myself!</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dcf6iflvy4ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1e9piho</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Nails by my bestie</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2i10br82y4ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1e9phpa</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>My first time doing gel x am I doing this right</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nr43cy8wx4ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1e9p8yo</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Honestly…. What do you think of these…?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjldvrg6w4ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1e9caie</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Please help me find what I'm doing wrong with my cuticles</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9caie/please_help_me_find_what_im_doing_wrong_with_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1e92f8c</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Happens Every Time</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzi22gur5zdd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1e93uey</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Terrible Pedicure :(</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e93uey/terrible_pedicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1e9ngow</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>I love my job 😍</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9ngow</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1e9nm56</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>My digital design v Inspo from u/wesjatta</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9nm56</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1e9ofob</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Classic Frenchies!</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rsnivwzbq4ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1e9o62i</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>I'm obsessed with this new polish from Glam Polish (Aus)</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9o62i</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1e9o37h</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>My engagement nails!</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9o37h</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1e9o2oe</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>I'm obsessed with these🩷😍</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9o2oe</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1e9ncki</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>What type of to glue for tips?</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9ncki/what_type_of_to_glue_for_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1e9b9vd</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Can someone please help me find this pretty nude color?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75nmqu21w1ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1e95r6d</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>peel off base on top of builder gel?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e95r6d/peel_off_base_on_top_of_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1e95euj</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>is it bad i want to give up doing nails?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e95euj/is_it_bad_i_want_to_give_up_doing_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1e9507k</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Itchy after Gel </t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9507k/itchy_after_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1e9id80</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Toenail shape</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9id80/toenail_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1e9ja99</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Tried press-on for the first time as a nail-biter... I have a lot of questions</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9ja99/tried_presson_for_the_first_time_as_a_nailbiter_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1e9n0x9</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Letting My Nails Grow: Week 7</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ii7dqvbag4ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1e9jise</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Allergy - I think my friends nail girl is ruining her nails!</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9jise/allergy_i_think_my_friends_nail_girl_is_ruining/</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1e9mxb2</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>switching from gel to acrylic</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9mxb2/switching_from_gel_to_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1e9mhg1</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Essie Primp &amp; Powder vs Lilacism</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9mhg1/essie_primp_powder_vs_lilacism/</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1e9mg5f</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is adventurous </t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gjj1n33c4ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1e9md16</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shiny </t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9rsmodgb4ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1e9mazq</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you like them or not? Brown </t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ckqagd3b4ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1e9ltgb</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>What do you think of this old green?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xmuxu7j74ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1e9lsxf</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>An excellent baby boomer</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4steaoif74ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1e9lkf7</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Recent set (I probably did to early) on myself 🥰</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9lkf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1e9lch1</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Fresh fill in!! 💙💙</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etpra65644ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1e9jdh9</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>idk if i like my nails</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9jdh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1e9jarm</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Birthday Set</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9jarm</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1e9j2bp</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Haven‘t done nailart in a while </t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xapzcu2sn3ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1e9dy2p</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Custom Bridal Set</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9dy2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1e9f87g</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Builder gel issues</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9f87g/builder_gel_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1e9fkoy</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Help, how do I get gel off and leave the acrylic in tact?</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8njkdxvx2ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1e9gsb8</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Difference between Hard Gel and Dip Powder - which is better for my needs/trip to Europe?</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e9gsb8/difference_between_hard_gel_and_dip_powder_which/</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1e9imia</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>the encapsulated ones are my favorites</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cq660l0jk3ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1e9hsyl</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Nail shop help! (UK)</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9hsyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1e9hp7t</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Moldy fruit set I did! </t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9hp7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1e9hmbw</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>New set ‘Punk’ part VI</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9hmbw</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1ea1744</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>My attempt on fishing lure nails</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ea1744</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1ea0nou</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Got gel w/ powder multi chrome finish</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ea0nou</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1ea0d0f</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Lavender Haze</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ea0d0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1e9z29x</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Creme Skittle Nails 🧡🍮💜</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxyua78z57ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1e9vb3p</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>So I ordered some bottles to decant some polishes…</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e9vb3p/so_i_ordered_some_bottles_to_decant_some_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1e9y87l</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Yall I've been caught 🤣</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rufxwqmx6ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1e9xmi8</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>I decided to try something new</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9xmi8</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1e9xhrg</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Even "natural" colors are so fun!</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9xhrg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1e9xdqu</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Polish-making supplies in Canada (like glitterunique)</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e9xdqu/polishmaking_supplies_in_canada_like_glitterunique/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1e9s6kd</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>lucky jelly</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2e0nenwh5ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1e9wto0</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI Kyoto Pearl vs E&amp;M Ballet Slippers </t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9wto0</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1e9wohc</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>That's your go-to topper, the one that looks good over everything?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e9wohc/thats_your_goto_topper_the_one_that_looks_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1e9w8io</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>how much of a n00b am I that I'm impressed by current products compared to products of decade(s) ago?</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e9w8io/how_much_of_a_n00b_am_i_that_im_impressed_by/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1e9vg6a</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Behold the gold!  🙂</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/22-7-2024-2dCCPlI</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1e9v05c</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summery Nails </t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6n3tqopr46ed1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1e9uz9y</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Can someone suggest me a dupe for Dior Nail Glow?</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e9uz9y/can_someone_suggest_me_a_dupe_for_dior_nail_glow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1e9uw47</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Highline featuring my broken nail 🪲</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9uw47</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1e9unyw</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Chiffon 💕</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzo4z6yv16ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1e9t9ms</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Neon vibes - it's giving summer </t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9t9ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1e9sh37</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Base for bumpy nails</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e9sh37/base_for_bumpy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1e9sa68</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Sassy Sauce “Shimmy Shake” after camping</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9sa68</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1e9s3vu</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Sea Glass nails</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9s3vu</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1e9rh3z</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>perfect color for the pool! 🩵☀️</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nizqsgagc5ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1e9r77j</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>🎨Color Wheel Series: Sage + Army Green🎨</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9r77j</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1e9r2h0</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Some of my manis this summer ☀️</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9r2h0</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1e9r1gg</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Is there a gentler way to take off gel polish?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e9r1gg/is_there_a_gentler_way_to_take_off_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1e9qarb</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>A very specific request</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e9qarb/a_very_specific_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1e9q2fp</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Partner picked it out</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9q2fp</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1e9ph2z</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Electric Summer by ILNP (PR/Ad) </t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9ph2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1e9p5b8</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice - oil, peeling nails </t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e9p5b8/advice_oil_peeling_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1e9okhy</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Lyn B Even Broken Bells Will Ring ✨</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9okhy</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1e9odvc</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>What's your favorite base coat that makes your mani last long, that DOESN'T contain polyvinyl butyral (so not Orly Bonder)?</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e9odvc/whats_your_favorite_base_coat_that_makes_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1e9ocii</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Two ticks and no dog </t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9ocii</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1e9o5f3</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rainy Day for a rainy day! </t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/namzojlco4ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1e9n1r1</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Holo over holo ✨✨</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9n1r1</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1e9m1na</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>RL Rule Updates</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e9m1na/rl_rule_updates/</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1e9lvcy</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matching my Car Today </t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9lvcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1e9ke22</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Nail art attempt</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97e4mt7dx3ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1e9k6lt</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Pandemonium 🔥</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9k6lt</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1e9k3gr</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer Transience ✨</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0nginqj8v3ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1e9j4t0</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Summertime and the livin' is easyyyyy (except for bad gel removal)</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9j4t0</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1e9izke</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Withdrawals</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e9izke/withdrawals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1e9ixj7</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Sunset skittle 🌅</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9ixj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1e9ii6o</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Request: low chemical polish</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e9ii6o/request_low_chemical_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1e9igcs</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Sparkly Shimmery Chunky Teal Blue Green Goodness</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9igcs</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1e9i3fu</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>🌴✨️Miami Vice Vaporwave✨️🐬</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9i3fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1e9hy2t</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Barry M mini haul!</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rk8i0brif3ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1e9gtrt</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Polyvinyl Butyral</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e9gtrt/polyvinyl_butyral/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1e9gphq</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DVN - Nostalgia </t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i8thfrid63ed1</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1e9ex9f</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>away from home mani 💜</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4j2p7enws2ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1e9euop</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>OKAY MOONCAT, I like you!!!</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9euop</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1e9epwo</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>12 days later, my first chip 🥲</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sto9zag9r2ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1e9e8qo</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Mooncat Acidic + Blossoms Firebreath 🧡🩷</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4rx7wkeen2ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1e9dtaj</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>BKL “God of Idiocy” with some macro fun</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydv5fz9sj2ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1e9djhx</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Witchy skittle</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4hu0lwcih2ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1e9dad7</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This color just makes me feel powerful and badass </t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9dad7</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1e9cey6</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Spending my office lunch break thinking about ice cream… 🍨</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqdigntj72ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1e9auzc</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cinderella blue russian manicure 🩵✨ (swipe for silly pics) </t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9auzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1e9ahpj</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e9ahpj/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1e9a1of</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>I had never given yellows a proper chance, but it turns out I love a good sauv blanc on my nails too!</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yp5yp420i1ed1</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1ea1968</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Did this practice set come out okay? Beginner nail artists 💕💅</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ea1968</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1ea0r13</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gorgeous summer nails </t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ea0r13</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1e9ykm0</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>🍋 Lemon Nails</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cem7o6yy07ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1e9yi9i</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>1st Nail Set</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w40asp9b07ed1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1e9xhvt</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Shorties</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9xhvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1e9xdmu</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t xml:space="preserve">some recent sets of mine </t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9xdmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1e9w346</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Okay but these on a date 😌💅 (done by me)</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ipcmu6hzd6ed1</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1e9vtjr</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>150USD Bubble bath bomb nail!</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9vtjr</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1e9voxh</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Struggling with isolated chrome. </t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9efh2pioa6ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1e9svju</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Under the Sea🐚</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9svju</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1e9qut2</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Apex legends nail art 💖 hand painted by meee 🥰</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76lwewit75ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1e9orgm</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>a very simple design 🩷✨️</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6sqjefos4ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1e9ok4x</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>3D model gel</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1e9ok4x/3d_model_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1e9ig0e</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>First timer with builder gel</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qozjd978j3ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1e9f8xz</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Newest Design ❤️</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2fqxyrfdv2ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1e9a90d</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Demon slayer Nezuko! nail art✨ this is how my first commission went🥹💕</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e9a90d</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1e99m9x</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Glass/Metal Nail Stands</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvji23jpc1ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jul 24 08:09:14 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_28.xlsx
+++ b/data/2024_07_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C478"/>
+  <dimension ref="A1:C636"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8559,6 +8559,2692 @@
         </is>
       </c>
     </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1eavapr</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Guess what it is?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4sx12ju4fed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1eav98y</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you put regular gel polish over BIAB and will this help my nails last? </t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eav98y/can_you_put_regular_gel_polish_over_biab_and_will/</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1eaul9u</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Dark Pink with Purple Chrome 🩷💜</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eaul9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1eauj5b</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>I overfiled my sidewalls right? Any tips?</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cwe5uyvveed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1eaqh3y</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My latest press on set, all hand painted by me! arisnailartistry on instagram </t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4belnjmpded1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1ear163</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vulnerable post </t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ear163</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1eatdvz</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to get press ons to stay </t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eatdvz/how_to_get_press_ons_to_stay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1eatic7</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Is the gap too big?</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eatic7</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1earwgo</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Nail polish color help</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1earwgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1easfo9</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>70's retro green kitchen inspired nails 💚</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1easfo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1eas8mh</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>My nails 🩷</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjzofm8i6eed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1eas86b</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Is there a way to file my slightly crooked nails, to look more straight?</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fzy4gwhd6eed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1eas3p9</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>any recs for gel x nail tips that are exactly this size and shape?</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eas3p9</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1earw0z</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Cute Two Color Aura Nails!</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1earw0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1eaqi1o</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>first time doing french tips!</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eaqi1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1eapsli</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Birthday set</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrbm6ianjded1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1eapqpd</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>First time Gel X 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/atk9kba7jded1</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1eaplsq</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>New set today 😍</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kc9z24o2ided1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1eapl8k</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Birthday nails I did on myself💗</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3t88synxhded1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1eapiph</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Best Friend did my nails - I think they should go for their license !</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sefho9u5hded1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1eapein</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Let me share my recent favorite nail style!</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eapein/let_me_share_my_recent_favorite_nail_style/</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1eaouv2</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>a perfect fill 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h07l5kvgbded1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1eaokso</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Nail strengtheners under gel?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eaokso/nail_strengtheners_under_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1eaogx0</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>I love them too much</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oml8dj9w7ded1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1eaoft8</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Birthday Nails!</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eaoft8</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1eamzrf</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Is this… good?</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eamzrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1eanwig</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Is there a good way for my nails to not look like I stuck them in a garburator after removing press ons?</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oljioh093ded1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1eanbw3</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>First almond gel set</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/den2ia3kyced1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1ean2c1</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Fresh set!!</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8j6mekjfwced1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1eampra</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I hate feet, but these colors do enhance them. Kiss Impress Feelings and Bubbly. </t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zh7dwwontced1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1eamfq3</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>3D gel art effects with regular polish! (First attempt lol)</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eamfq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1eameq1</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Acrylic kit recommendations?</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eameq1/acrylic_kit_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1eam7ca</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>I think I have bad luck :/</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eam7ca</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1eallb8</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Looking for tips - nail breakage and keeping nails healthy</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eallb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1eakmz5</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>im planning on getting biab on my fingernails and toenails what do i pick (all inspo photos from pinterest)</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eakmz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1eakzl2</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Nails of the week!</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80hfeitcgced1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1eakuws</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>🩷💙</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eakuws</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1eakm1x</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Spooky nail set for a Halloween convention</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eakm1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1eakjfh</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>ILNP - Deep End</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eakjfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1eakaix</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Can gel nails not harm the nail?</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eakaix/can_gel_nails_not_harm_the_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1eaha8o</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>y2k inspired.. thoughts?</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dlhvw9kpbed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1eajtu4</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>my first attempt at ombre</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29tnz94k7ced1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1eajfc5</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>My nail tech is insane for this</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hiio3xs4ced1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1eait49</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Stained glass set I did on myself 🥰</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eait49</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1eaisfm</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>long (but small) coffin nail tips?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eaisfm/long_but_small_coffin_nail_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1eai4fv</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel Colour Change on Acrylics? </t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eai4fv/gel_colour_change_on_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1eahzbm</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Accidentally Starbucks color</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eahzbm</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1eahi40</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>almond or round shape?</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eahi40</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1eag9vm</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Tips PLEASE 😩</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37x2mlxbibed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1eagoqj</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>How can I take off gel polish top coat off dip nails without ruining them?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eagoqj/how_can_i_take_off_gel_polish_top_coat_off_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1eah0u3</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>I love them</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fz10ndpnbed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1eagtbq</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Why doesn’t blue suit me?</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eagtbq</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1eaguj4</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>New butterfly nails 🦋</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z50zcrtfmbed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1eagqqi</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Regular Polish Over BIAB? </t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eagqqi/regular_polish_over_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1eagepl</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Found a perfect nude for me!</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eagepl</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1eagekl</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>New nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eagekl</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1eagbyg</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can't pick my nose but it's worth it </t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eagbyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1eafwit</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>The checker one is my fav &lt;3</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gow7vjgpfbed1</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1eafw1r</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>The checker one is my fav &lt;3</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9pwr7cwlfbed1</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1eafw44</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>pink &amp; sparkly summer nails</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eafw44</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1eafq5f</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>pink cat eye stilettos ! 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eafq5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1eafoky</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>New color, new me!</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32taqen3ebed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1eafc67</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Need advice on "plain" press on nails</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eafc67/need_advice_on_plain_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1eaf26s</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Long frenchies✨</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eaf26s</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1eaek2y</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Safe way to remove chrome off LCN?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eaek2y/safe_way_to_remove_chrome_off_lcn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1eaefwb</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>My first attempt at poly gel</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfwqvr915bed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1eaefw9</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Did a set for my upcoming birthday this weekend 💅🏾🎉</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eaefw9</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1ead23z</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HELP I need a nail tech </t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ead23z/help_i_need_a_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1ea16lu</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Think my nail guy filed too hard on my actual nail? 🥲</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfn8ykk2u7ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1ea2x3n</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>flexible nail colors/designs?</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ea2x3n/flexible_nail_colorsdesigns/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1ea311d</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>How do you put on gel nails that already have a design?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ea311d/how_do_you_put_on_gel_nails_that_already_have_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1ea4dr2</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Should I change my nails for graduation?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ea4dr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1eae2g5</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>I'm in love with this set but the tech didn't built the gel  apex up like im used to so I am worried they will break! wwyd?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eae2g5</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1eadwiv</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Help me find petite press on nails</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eadwiv/help_me_find_petite_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1eadx8c</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>New Set! 🌊✨🐚</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/skn31j2e1bed1</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1eadpbt</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>do you guys like my y2k nails❤️😁</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eadpbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1eadp1n</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>6th set</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eadp1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1eadotd</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>do you guys like my y2k nails❤️😁</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eadotd</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1eadich</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Is this worth $70?</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eadich</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1ead1lb</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Cherry ❤️🍒</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jexchla1vaed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1ea4asq</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Where to source long toenail press ons? </t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ea4asq/where_to_source_long_toenail_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1eaaxzp</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Somewhat upset about Nail News…</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eaaxzp/somewhat_upset_about_nail_news/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1eab940</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Brand Komilfo?</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eab940/brand_komilfo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1eacarz</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>First time in forever</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eacarz</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1eac3px</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>fave set to date</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eac3px</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1eabs0s</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>New set ‘Punk’ part VII</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eabs0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1eabpeu</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>After years of plain nail polish I am pleased to announce I am back on my nail art game 💅</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2ws8dmglaed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1eabg0q</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Press ons from Amazon</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eabg0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1ea7z6j</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Freestyle nail inspo 💖</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ea7z6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1ea9nt4</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Obsessed with this color</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uep89mxu6aed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1ea9m22</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vibrant magenta, I’m in love 💖 </t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ea9m22</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1ea80lw</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Accidentally matched with my friends vape</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipqlr6e6u9ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1ea7v88</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Glue on Nails Question/Advice!</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ea7v88/glue_on_nails_questionadvice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1ea7jzr</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>First time trying to do acrylics at home, but the powder creates like a foam instead of a bead? Is this normal? What am I doing wrong? Please be nice 😭</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2ngcyhdq9ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1ea796w</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Holo Taco Barista Bundle</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ea796w</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1ea71zh</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t xml:space="preserve">More colours, more! </t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ltdieobm9ed1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1ea6loi</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Mellow Yellow</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ea6loi</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1ea69w8</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>I love this colour 😍</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ea69w8</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1ea63gf</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3abdqtmd9ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1ea5cth</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Fun little set for my birthday month</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8vpo4qwa69ed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1eavoi4</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JL Lacquer // God of Mischief </t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eavoi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1eau8do</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Black Sand Gels</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcogfhhcseed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1eargk6</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>It’s giving asphalt chic</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eargk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1earajy</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Mani and inspo</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mf78j5s6xded1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1ear5yv</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>What is one nail polish finish or addition that makes you go, "oh, I NEED that polish"</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ear5yv/what_is_one_nail_polish_finish_or_addition_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1eapzuq</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Glitter leopard print!</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kv3t9pcalded1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1eapv8v</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>I'm not sure how I'm feeling about it just yet</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eapv8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1eaps10</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Layering Magnetics</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eaps10</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1eapgnn</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>A ghostly blue</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eapgnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1eapbv1</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In search of.. </t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ta2ci7ymfded1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1eapa44</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>ILNP - Carved</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eapa44</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1eaoutp</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>No such thing as too much polish, right?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eaoutp</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1eanrs6</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>It IS Electric!</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eanrs6</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1eamuj0</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>melancholic ripples ｡𖦹°‧</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eamuj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1ean092</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>This shade of purple 💜🤩</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7l3wet4zvced1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1eamzrr</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Tried to do ombre for the first time, failed catastrophically but kinda like it 😂</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsyj24ovvced1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1eamqpk</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>tips drying matte??</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eamqpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1eamkwm</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>I was hard on my manicure this week, so I touched it up - now my nails look like those blue caves in Iceland 💙💫</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eamkwm</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1eamet5</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you use a normal topcoat with thermal polishes? </t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eamet5/can_you_use_a_normal_topcoat_with_thermal_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1eam8y6</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>First attempt at 3D nail art using JUST Seche Vite top coat!!!</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eam8y6</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1ealmm1</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Newbie at French tips and water decals</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ealmm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1eallol</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Am I missing something here or did I get tricked by the photos…</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eallol</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1ealjr6</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Recommendations for flaky splatter toppers</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ealjr6/recommendations_for_flaky_splatter_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1ealf4g</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Cat approved Mani</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhf6m98mjced1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1eakfpb</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>ILNP - Deep End</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eakfpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1eajwbj</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Got my hands on (some of) the HT thermals</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eajwbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1eajir3</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Can’t stop staring at my nails!</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eajir3</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1eaj996</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>First Timer</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eaj996/first_timer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1eaik3i</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Obsessed with Essie Cactus Jelly 🤩</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wh1rhw3mybed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1eahcps</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Has anyone with Raynaud's done thermals? How did it turn out?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eahcps/has_anyone_with_raynauds_done_thermals_how_did_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1eaeems</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Skittle </t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jb94u2pv4bed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1eadfcn</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Can’t decide if I love or hate these.</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9785wdsxaed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1eaco2w</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Layering fun with thermals!</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/balhgfuvraed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1eace8t</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matching for storytime </t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h69yltfeqaed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1eace6n</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Lunar Skystone</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eace6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1eabxwy</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Electric Summer comparisons to other ILNP shades by sbrown.nails on IG</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eabtqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1eaajx9</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Different IBD gel ingredients?</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51f3fwe9daed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1eabhub</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>New case</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eabhub</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1eaatmj</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Milk Tea, or Orange Creamsicle?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eaatmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1eaa2bl</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t xml:space="preserve">But do Aliens believe in me?? </t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eaa2bl</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1eaa05v</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>90s Windbreaker Chic</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eaa05v</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1ea8rpp</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Has anyone experimented with conductive materials that turn your nails into a touch screen stylus?</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jtf2uwn30aed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1ea8e8h</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Replacement brushes?</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ea8e8h/replacement_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1ea7zv9</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Holo Taco Rage Bait</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ea7zv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1ea6rnp</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Opi bubble Bath and Sweetheart Dupes</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ea6rnp/opi_bubble_bath_and_sweetheart_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1ea6jmr</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Searching for a nude</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ea6jmr</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1ea3y1x</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Press ons on ski slope nails?</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trstqu13r8ed1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1eaqdwr</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My latest press on set, all hand painted by me! arisnailartistry on instagram </t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xrc03ghtoded1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1eaoixv</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Birthday Nails!!</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eaoixv</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1eaobe4</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>What do you think about my nails? 🐆🍒✨</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcc03kjq6ded1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1eao471</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Que tal las uñas que me hizo mi vecina 👌🤩</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9m0y7215ded1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1eajse6</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sparkle ✨️ Decals </t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eajse6</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1eajb2f</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>How can I accomplish these nails</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/C9lS7V7SpYE/?igsh=MXVkazQ3cjlmNHJ1eQ==</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1eafeyw</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>all pink😍</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctxywz37cbed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1eadsum</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1eadsum/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1eaas6v</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Curious about foils</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eaas6v</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1ea9ays</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Nail charms/rhinestones</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ea9ays/nail_charmsrhinestones/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1ea89h6</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh Pink &amp; Red Set. </t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2lslwig9w9ed1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jul 25 08:09:57 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_28.xlsx
+++ b/data/2024_07_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C636"/>
+  <dimension ref="A1:C813"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11245,6 +11245,3015 @@
         </is>
       </c>
     </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1ebmw0e</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Let my 15yr old do my non dominate hand for the first time</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axllrqgknled1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1ebmoap</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you reuse press on nails? </t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ebmoap/can_you_reuse_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1ebmezm</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Glow in the dark Fallout themed nails!</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xsnq28bniled1</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1ebmdkb</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>DIY Kiara sky gel is my go to!!❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fardhz59iled1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1ebm91l</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Sometimes I like classic</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmwn8icpgled1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1ebm615</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>First Time Gel X</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z926mhb3gled1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1ebkjjh</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I do my own Nails </t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebkjjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1ebk3sl</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t xml:space="preserve">classic red! </t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebk3sl</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1eblk9g</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Futurama Hand Painted Set</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eblk9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1ebl4fg</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Marvel Fans?</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebl4fg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1ebl2rf</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails who dis </t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebl2rf</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1ebkxi6</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>hello there! 💅🏾</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebkxi6</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1ebkvvu</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>BYEEEEEE!!!!</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tagk5i573led1</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1ebklg1</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Did my nails for the first time in awhile</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebklg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1ebk4xn</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got my nails done today !! I’m obsessed </t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4h9ep2hfwked1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1ebk3sm</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Current Nails 💅🏽</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azngmrf5wked1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1ebjllq</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Grandma’s wallpaper 🌹🌹</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wilplrdorked1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1ebiyir</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>little sis did my nails</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebiyir</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1ebirpl</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Birthday nails 🩷</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmmyxa1ekked1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1ebiorn</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>My sister did my nails 🥰</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebiorn</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1ebigqk</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Was I scammed</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxl1gayphked1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1ebhps6</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Nail inspired tattoo</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebhps6</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1ebi28h</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>First time trying Gel-X 🖤</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebi28h</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1ebhw8s</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Ready to see Deadpool and Wolverine!</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebhw8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1ebhgzv</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Got gel extensions in Japan, how to remove the coloring but keep extension?</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ebhgzv/got_gel_extensions_in_japan_how_to_remove_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1ebhgdu</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Iridescent nail with funky tips</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebhgdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1ebgko7</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Welp, I tried press ons for the first time ever, and I thought I did good until moisture got under them. How can I avoid this in future?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18o1wtqn1ked1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1ebfclq</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>New gel x set but cuticle problem</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ryur502sjed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1ebfilu</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>how to strengthen natural nails? also shaping tips appreciated!</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ebfilu/how_to_strengthen_natural_nails_also_shaping_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1ebfebo</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Gundam nails, anyone?</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebfebo</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1ebe8f7</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone recommend a pedicurist in the LA, CA area that would work on a fungus toe? </t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ebe8f7/does_anyone_recommend_a_pedicurist_in_the_la_ca/</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1ebf5rl</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Latest set I did</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebf5rl</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1ebf07y</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ad6yti8ipjed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1ebeaxr</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>I posted these on my TikTok and ppl commented ‘looked at my nail tech and sighed’😂</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebeaxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1ebeq01</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>I like ? 😍</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nx4d06sanjed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1ebeo0m</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’ve been declawed! Gel polish on natural nails </t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4i0fxlumjed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1ebenc4</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cheap press on nails. </t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3p9ou9jpmjed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1ebeeq4</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>new press-ons for the last stretch of summer</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebeeq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1ebe6fv</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>(not my work) haven’t gotten a full set in years. loving them!🥰</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ocksg6qrijed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1ebdhcx</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>My Girlfriends Nails</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebdhcx</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1ebdbnw</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>ISO recs for dark nail polish (black but kinda red, for example)</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ebdbnw/iso_recs_for_dark_nail_polish_black_but_kinda_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1ebd41i</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Is there a way to do 3d nail art with SOFT builders gel?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ebd41i/is_there_a_way_to_do_3d_nail_art_with_soft/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1ebcu8s</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Cajun Shrimp 🦐❣️</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ga76bl1x8jed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1ebcamt</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Summer sets are my favs always</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvhzndtz4jed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1ebbcxc</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Alternative removal methods for gel-x</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ebbcxc/alternative_removal_methods_for_gelx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1ebandt</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Getting acrylics for the first time.</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ebandt/getting_acrylics_for_the_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1ebbu19</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>anyone know what this is used for?</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebbu19</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1ebbk8r</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer set </t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebbk8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1ebbh1s</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>New press ons thanks to the girlie's in here 😛 obsessed 😍</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jruh45f0zied1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1ebbfrb</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Kokoist retention FTW</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nqtvl33ryied1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1ebb7dk</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Want to do my own nails: Suggestions? </t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ebb7dk/want_to_do_my_own_nails_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1ebar7a</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>🩷 ILNP Pixie Party ✨🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebar7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1eb9yxo</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Rossi Nails no longer delivers to USA: Best alternative?</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eb9yxo/rossi_nails_no_longer_delivers_to_usa_best/</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1eb9vfe</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unsure if this colour suits my skin? </t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5yvq7f7gnied1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1eb9pew</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Cinnamoroll nails</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kbxgsm7mied1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1eb9g0n</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Salon tickle torture </t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eb9g0n/nail_salon_tickle_torture/</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1eb9cg5</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>How to get BIAB off at home, with easily available products?</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eb9cg5/how_to_get_biab_off_at_home_with_easily_available/</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1eb8t1a</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>I need advice!</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eb8t1a/i_need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1eb96a4</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Love my nail girl! 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wrjaff5eiied1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1eb7tin</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>I cant decide which aesthetic to go for again! my last 3 sets</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb7tin</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1eb8lqn</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>look this art girlies, the artist is @gothic.ib</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb8lqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1eb7wyl</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Neon summer! </t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35e8bo2a9ied1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1eb7rhn</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>love this design ✨️</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpc36jp78ied1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1eb7ovo</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>cute strawberry set I did last night! builder gel with tips</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sx0yelql7ied1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1eb7njk</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Meet the Mohawk - new set ‘Punk’ part VII</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb7njk</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1eb7mdq</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Chrome blobbies</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb7mdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1eb7bia</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Sea shell nails!💅</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gh93ry705ied1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1eb6zvo</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>QUESTION: What is a nail shape that suit me?</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb6zvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1eb6u0z</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my first set of press ons :) </t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nqn3o25k1ied1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1eb6tpt</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I finally figured out how to make gradients with polish </t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb6tpt</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1eb6k1r</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Do I just wait for my hard-gel nail extensions to grow out?</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eb6k1r/do_i_just_wait_for_my_hardgel_nail_extensions_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1eb6q8a</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb6q8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1eb6i9f</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>I followed your advice and decided to do almond nails! I always thought they looked bad on me because I had large nails</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb6i9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1eb5py7</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Return to acrylic</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eimao80jthed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1eb5n1a</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>First time making gel nails!</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txo9yeexshed1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1eb5kyv</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>New diy set</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb5kyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1earms4</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>How to Choose a Nail Tech?</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1earms4/how_to_choose_a_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1eb36ts</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Drag queen Laganja Estranja inspired nails I made</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb36ts</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1eb379b</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Is this worth 100 dollars?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb379b</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1eb3lth</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday to Greece next week! Does anyone have any inspiration for my nails? </t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb3lth</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1eb55ee</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>I'm a noob but painted my nails last night and am tickled with them</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijvjewmcphed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1eb4gkp</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Gyaru Inspired Nails (to complement red/ivory/black outfit &amp; accessories) 🎀 ✨️</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb4gkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1eb4qcy</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Alice in wonderland set I did 💅</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9ij3fiamhed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1eb4fnl</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Finally found a golden polish that I love. What do you think?</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1feh683khed1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1eb3l2a</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Which shape looks best for me?</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb3l2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1eb3kyy</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Using half tips with curved nails?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eb3kyy/using_half_tips_with_curved_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1eb36nj</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Good quality gel polishes? Milky white</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eb36nj/good_quality_gel_polishes_milky_white/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1eb1kmj</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Was admiring the nails I gave myself when out of nowhere...</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb1kmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1eb2tkh</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Opinions? I just got them done and I don’t know if I’m being too picky or not.</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb2tkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1eb1ve0</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think about my new nail??? </t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9nrsji3u0hed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1eb1t1a</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Why won't nail glue work for me?</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eb1t1a/why_wont_nail_glue_work_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1eb0wpo</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Brat summer :3</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cd1d4tb1tged1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1eaz3mz</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>What nail trend do you not get the hype about?</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eaz3mz/what_nail_trend_do_you_not_get_the_hype_about/</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1eaz24c</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I went for a fruity glitter encapsulation moment! </t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eaz24c</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1eaybka</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Summertime and the livin' is easy🍒✨️🦦</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eaybka</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1eaxvtw</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love a basic set 🤩 </t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/igmrpgnnzfed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1eax0ed</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Are they perfect match?? What do you think?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eax0ed</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1eaw7i5</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new clawz </t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eaw7i5</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1eaw0y8</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Nail filling tips please.</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eaw0y8/nail_filling_tips_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1ebmt9p</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling discouraged </t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ebmt9p/feeling_discouraged/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1eblno4</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Stained glass nails</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eblno4</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1ebkk76</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Neon gradient + clear and black watermarble 🦜💙</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n97avrd80led1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1ebk1b5</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>NYC Red Velvet Rope</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebk1b5</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1ebjqtp</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Best primary yellow cremes?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ebjqtp/best_primary_yellow_cremes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1ebitkk</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>velvet nails !!</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebitkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1ebit36</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>velociraptor by mooncat 🦕</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2izuuc9qkked1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1ebislv</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>What should I do with my gel polish?</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ebislv/what_should_i_do_with_my_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1ebi320</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Holo Taco?</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ebi320/holo_taco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1ebhvn2</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Ready to see Deadpool and Wolverine!</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebhvn2</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1ebhnhy</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Orly's Glass Act</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebhnhy</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1ebhd01</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Big chop!</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebhd01</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1ebh5ck</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>What A Catch</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4dn41pc6ked1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1ebguey</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Recreate?</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebguey</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1ebgopm</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Amuck Amuck Amuck! by Mooncat! whose ready for fall😁😂🙏🏼 i think i am ! don’t come for me 🤣🫣</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uaa81ldl2ked1</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1ebghhz</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thermals on short nails </t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebghhz</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1ebgcth</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Mooncat “replacement bottles” aren’t any better?!</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebgcth</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1ebgade</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>I'm loving this summery reddish/orange color!</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7il0ohdzjed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1ebfenh</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>ILNP Deep Space (over two coats ILNP Hush) ft. roomba</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2d3n7ah1sjed1</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1ebf394</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>So my nails matched my drink! (2+ years of consistent manicures and poses still look awkward! Lol!)</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebf394</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1ebefza</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>What brands do you recommend? (New to nails)</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ebefza/what_brands_do_you_recommend_new_to_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1ebe8xk</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>My latest LynB haul</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebe8xk</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1ebdtpx</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>DVN "Hose Water" = Summer Vibes!</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ebdtpx/dvn_hose_water_summer_vibes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1eb7alz</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Is this a nail fail?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb7alz</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1eb88oz</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>How to get nail polish out of bed comforter?</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxk9wekhbied1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1eb95n6</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>BKL Goddess of Rot</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb95n6</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1ebcest</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Now Go And Don’t Look Back</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebcest</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1ebbv5r</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Moody Matte Mani</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cw4trt1w1jed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1ebbk4w</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>First Try</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rvj5m1skzied1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1ebaujo</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Fancy Gloss “Arcstrider”</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebaujo</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1ebaqol</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>🩷 ILNP Pixie Party ✨🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebaqol</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1eb9spi</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Can I paint over China Glaze Fast Freeze?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eb9spi/can_i_paint_over_china_glaze_fast_freeze/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1eb4kqf</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you store your polish and tools? </t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eb4kqf/how_do_you_store_your_polish_and_tools/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1eb91j8</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Nail “art” ft. Clambake sandwich</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akxgikchhied1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1eb8ex0</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>DNV' "Refracted Light" / FUN Lacquer / Magnetic top coats?</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eb8ex0/dnv_refracted_light_fun_lacquer_magnetic_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1eb7uwj</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>The Fluffiest Blanket</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb7uwj</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1eb6xui</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Icy blue chrome powder, my 2nd attempt at doing my own gel nails. I get so shaky. Hope I can learn to paint inside the lines better with time! </t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb6xui</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1eb5xpw</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Really like how these turned out!</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l15jnms3vhed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1eb5ttz</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JL Lacquer // God of Mischief </t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb5ttz</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1eb5ngk</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Made a Summer Thermal</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5weowbj0thed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1eb4wiq</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Banana Cream Pie vibes?</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb4wiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1eb4lrh</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Blah</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb4lrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1eb4egl</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>I have a weak spot for purples</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb4egl</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1eb4a4s</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>How do I mix in this glitter stripe?</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1krjtumzihed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1eb3h6j</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Ohh so sparkly orange</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb3h6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1eb2wah</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>I am so over my polish wrinkling at the tips 3+ hours after finishing my manicure.</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlw3tnet8hed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1eb209n</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Sassy Sauce “The Midas Touch” + updated Shimmy Shake</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb209n</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1eb18h0</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Gosh I hate poetic descriptions</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eb18h0/gosh_i_hate_poetic_descriptions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1eb09tb</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>I work in a historic library and tried to do "old book" nails</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb09tb</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1eazz2n</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>A pleasure for the tips</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eazz2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1eaxvut</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Fancy Old Plate Nails</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eaxvut</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1eaxqa5</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>My love/hate relationship with speckled polishes</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7i5s25mxxfed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1ebm0iz</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Soft blush 3d nails 🧉🌺🌸 IG adpnail 💕</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebm0iz</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1eblyyh</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Futurama</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eblyyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1eblwnv</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Nails inspired by the cyclops saga from epic: the musical :)</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eblwnv</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1eblejz</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Glow in the dark Fallout themed nails!</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fjjzf7gc8led1</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1ebgrcs</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>I'm in love 😍 by : @streetnailart</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7awois63ked1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1ebfqnz</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Tiny canvases, big art! Watch my hand-painted nail journey unfold. 🌟💅</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebfqnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1ebekmo</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Taking nail pictures be a struggle sometimes still fun though….I tried the rain drop affect on the thumb only. </t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebekmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1ebadxj</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>New to doing my own acrylics, here are some of my best designs!</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebadxj</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1eb7vtc</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Ive started making my own press ons :)</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb7vtc</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1eb7ssu</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>something simple and natural</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzuxpn8h8ied1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1eb7byl</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Frenchies done by me</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1m0aaqd35ied1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1eb6oxd</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>I did my nails myself, what do you think of the design?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3o7zq4bj0ied1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1eb6mfj</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>cyber gothic 👽</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb6mfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1eb6hd9</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>I miss my nails so much 🥺Should I have them done again? I made them myself</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb6hd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1eb5zzf</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Flame ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ke4itijkvhed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1eb5x31</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Galaxy Nails</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb5x31</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1eb5fm9</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Holiday nails - help!</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68dgynierhed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1eb54n0</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What I did today! </t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb54n0</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1eb53gq</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Need caviar bead advice</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m57ppwizohed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1eb4mrv</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I've done sushi and now breakfast nails what should the next food set be? </t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1yfczgtjlhed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1eb43qi</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>New to this but loving it! (And my cats love watching)</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb43qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1eb3aih</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did these last night. Flash vs no flash </t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7sr2y03sbhed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1eb2yku</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Summer firework 🎇</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eb2yku</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1eb1tko</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>What do you think abou my new nail? Its Go Yohan from manhwa Sign</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrbk694g0hed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1eaz36q</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Any Hazbin Hotel fans?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/huxjey0ccged1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1eayil2</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Rico Nasty KeyLime OG nails my 4th character nail art</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eayil2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jul 26 08:09:00 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_28.xlsx
+++ b/data/2024_07_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C813"/>
+  <dimension ref="A1:C978"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14254,6 +14254,2811 @@
         </is>
       </c>
     </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1ecia5t</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Stopped biting my nails, what next?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pmjj13sbhted1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1echvgi</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Can I put builder gel on a child?</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1echvgi/can_i_put_builder_gel_on_a_child/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1echi1e</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Summer vibes 🩷🧡</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwakyim18ted1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1ecgz0a</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Summer blues</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecgz0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1ecgnwq</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Super short nails</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecgnwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1ecd3a2</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Overlay?</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecd3a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1eccryx</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel-X </t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eccryx/gelx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1ecen7v</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Strawberry Fields + Lilac</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9e56agr0dsed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1ecdt36</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Rainy summer nails</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1u4l62y4sed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1ecdeog</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you do to keep your nails healthy with constant water exposure? </t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ecdeog/what_do_you_do_to_keep_your_nails_healthy_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1ecd3d9</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>⭐️ 🐠</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zkf1zoyeyred1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1ecctyu</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>made by me</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ss1d51v1wred1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1eccndg</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Tons of space between gel tips and natural nail. Is this normal?</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eccndg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1eccn36</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Beginner tips please 💅</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eccn36/beginner_tips_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1ecclye</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails keep popping off! Help! </t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iakomk82ured1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1ecclhj</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>My second ever gel manicure! Using builder gel and freehanded french tips</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgvxoaqxtred1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1eccksr</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Finally found a bright red that I like against my skin tone 🥰</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eccksr</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1ecccyf</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Lots of fun nails lately 💫 structured gel manicures done with hard gel on my recent clients’ natural lengths 💘</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k3m2v0ehqred1</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1eccd0x</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Finally did it</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6hagxdtrred1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1ecc4sw</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>My Golden Birthday set! I usually don’t go for gold but it was a must for the occasion✨</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecc4sw</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1ecc1vk</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>worth $80?</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fwyiofwwored1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1ecbku1</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>What nail chrome powder is this?</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3k1fu5mkred1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1ecb8wf</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Dupe for Sally Hansen Chill Frost??</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hhuwnxrhred1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1ecb6dw</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gym girls pls don’t use the pressons </t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecb6dw</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1ecb1zr</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Got my nails done</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecb1zr</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1ecb11v</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>first time doing nail art!</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecb11v</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1ecazp6</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Orchid 🦓</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hp6krxnkfred1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1ecat51</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>What do you think? Took me 3 hours 😭</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecat51</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1ecastg</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Pink radiance !!</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecastg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1ec7zoo</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>First time salon help for someone who picks/bites their nails?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec7zoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1ecan42</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>My wife is so talented. Just looking for some feedback. Thanks</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kp1za9mkcred1</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1ec6u2g</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These nails are making a statement, and i love it.  </t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbmelqeaiqed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1eca1yp</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>I am a guy, I just got these nails done for a wedding. What do you think?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9aea4ger7red1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1eca8yl</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Aside from being crooked, is the shape right or wrong for coffin? I need feedback to know what to tell the owner when I go back for a redo.</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/njbgfsna9red1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1ec94j8</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Too long for square French ombré? Does this look odd?</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mpp3v7j60red1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1ec92g9</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing almond and I love them!! </t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jknd66spzqed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1ec8d22</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Jelly red nails</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x70y9g2buqed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1ec8482</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Why did the nude on my French change colors?</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kliaevcsqed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1ec7ta1</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>tried doing nail art for the first time, Moon Knight and Tigra themed 🌙 🐅</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec7ta1</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1ec7nf6</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Nail set redux!</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec7nf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1ec7e5j</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Mommy/daughter nails</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ec7e5j/mommydaughter_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1ec7abs</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>first ever practice set!</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cni3y9hzlqed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1ec5tsf</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Hi, I have really messed up nails from an injury. How can I make them look better? :)</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec5tsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1ec6cd1</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Do you think this nail set would look good with printed flowers on it? 🥹</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18yfflhreqed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1ec61h3</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My girl did her thang </t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec61h3</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1ec5qxp</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>A little bit of shine</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0dadtu6daqed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1ec5lu1</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>what do you guys think?</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dep3avua9qed1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1ec466r</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Fight of my life but I did it</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec466r</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1ec58gq</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Daytime office, night shift 💅🏼</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k3bqf80j6qed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1ec54d5</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed 💕💅🏾 </t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnd5lzlo5qed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1ec50p3</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I loveeee this set I made, it screams summer 😍 </t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfoimoew4qed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1ec4npd</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Question about sizing for Lovful press on nails</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ec4npd/question_about_sizing_for_lovful_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1ec4j3r</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Is Etsy good for press ons?</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ec4j3r/is_etsy_good_for_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1ec2n2g</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>(man)icure</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ec2n2g/manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1ec33ot</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Finally did my nails after 6 weeks</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/50m011m5rped1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1ec316q</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>2024 Summer Nails🩵</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec316q</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1ec2vqy</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My summer of fruity nails </t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kpohjlckpped1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1ec2pdq</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>First time got professional gel nails</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9u2bp08oped1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1ec1cl5</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Thoughts on beetles nail kit?</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ec1cl5/thoughts_on_beetles_nail_kit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1ec0tey</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Switch up the shape?</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec0tey</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1ec0lul</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I said mermaid inspo and my nail tech ran with it. </t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdua64n49ped1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1ec2g4d</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Some froggies 🐸 3rd set I've ever made</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec2g4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1ec27hy</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh set, do they look good </t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q25f7w8okped1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1ec26sf</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>New favorite set!</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec26sf</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1ec23hd</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Nail tech who specializes in freestyles that capture my clients individuality ✨❤️</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec23hd</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1ec1t2d</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I too late for summer vibes? </t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gm17toqshped1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1ec0vk2</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>What is the most common color for nails in the month of August?</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ec0vk2/what_is_the_most_common_color_for_nails_in_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1ebzrzn</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Builder gel</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ebzrzn/builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1ebzkme</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Gel X Sizes</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ebzkme/gel_x_sizes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1ebz6bg</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summery yellow DIY nails </t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/610l3reoyoed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1ebyjrq</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>my natural nails with kapping 🥰</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ql7py1n2uoed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1ebyarr</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Did my own wedding nails 🤍</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebyarr</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1eby9uw</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sometimes, a classic black mani and a cuddly pup is all anyone needs </t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t05p7rp1soed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1eby61k</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Pink Chrome nails 🩷</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/if40wg88roed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1ebxlbw</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>My favorite set of the summer thus far</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebxlbw</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1ebxh1i</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what do you think? </t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebxh1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1ebx119</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>I’m so confused about this powder.</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnof3znzioed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1ebtnfn</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Blue gummy bears on all fingers</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2d7e4q5sned1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1ebwu6f</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>getting engaged within the next few months so i need to be prepared 😂</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7kiwb8ilhoed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1ebvldd</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>How soon would you wait to remove a gel manicure?</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ebvldd/how_soon_would_you_wait_to_remove_a_gel_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1ebubr8</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebubr8</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1ebu3k5</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>New sets!</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7lhtk33wned1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1ebt1u3</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Acrylics popping off</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ebt1u3/acrylics_popping_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1ebsuvr</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Nezuko nails, do you like it???</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0auun1rkned1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1ebsfuv</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Are these too thick?</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebsfuv</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1ebrxk5</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>8th set</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebrxk5</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1ebrraz</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>7th set... (and 7.5 😂)</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebrraz</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1ebq8to</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Look how cute ahhhh!</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebq8to</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1ebq8jw</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Criticism on this set?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qkz3hfarmed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1ebq172</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done yesterday </t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebq172</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1echltw</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat is neutral about the mani this time around. </t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pj9wbila9ted1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1ech9on</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Sand Viper ✨</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mau3n92b5ted1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1ecg4la</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Second Try - Pink this Time!</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2g9od7qgssed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1ecfedw</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Paradise - Buddy approved ✅</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecfedw</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1ecexah</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Polished For Days - Baja Blasted🌊💚🩵</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecexah</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1ecedrs</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Rate My Mani: ✨💙🩷✨ Spyglass &amp; Blush Money + Razzle Dazzle ✨🩷💙✨</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecedrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1ece7ll</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Love for shorties 🩵💜</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rfg04ep8sed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1ecd9zd</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Hope my coworker likes this set, my first ever</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/824pqwkzzred1</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1ecctre</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Can anybody recommend a (regular) nail polish in this shade of red?</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sise6hcyvred1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1eccf2f</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Gel girlie wanting to become a regular polish girlie</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eccf2f/gel_girlie_wanting_to_become_a_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1ecc9cj</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>The fairycore skittle of my dreams</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecc9cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1ecb6hz</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Dupe for Sally Hansen Chill Frost??</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9o3lnyz6hred1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1ec9zls</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Cirque birthday haul!!</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec9zls</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1ec9mnq</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>I’ve been playing around with layering and made the sunny yellow flakie of my dreams</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec9mnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1ec92ki</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Trying More Summer Colors!</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/es72fzyqzqed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1ec8w5t</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>messy but the idea is cute!! (i think)</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vy57ierbyqed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1ec8t4z</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Probably the sparkliest polish I own!</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec8t4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1ec7qc7</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Fair Maiden Polish - Tourmaline Dream</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec7qc7</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1ec6k2i</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first Phoenix Polish and omg, it's magnificent </t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec6k2i</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1ec5rqo</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Chanel Rouge Noir Dupe</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ec5rqo/chanel_rouge_noir_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1ec21rg</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Opinions? I’m just starting out and struggling to find things affordable and still good. Would really appreciate gel polish brand recs too❤️</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec21rg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1ec1tay</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Substitute for Pink Gellac's 166 Vintage Nude</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ec1tay/substitute_for_pink_gellacs_166_vintage_nude/</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1ec1ota</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Help! It’s not sticking!</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ec1ota/help_its_not_sticking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1ebutr0</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Thoughts on how to use this polish that I don't like?</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gtkdqcm52oed1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1ebqtz1</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Is it normal that thermal nail polish takes way longer to dry?</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ebqtz1/is_it_normal_that_thermal_nail_polish_takes_way/</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1ec4xkt</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Love some good velvet nails</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec4xkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1ec4lde</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Holo Taco Thermals</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec4lde</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1ec4ikw</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Streaky yellow lacquer</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ec4ikw/streaky_yellow_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1ec4hrn</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>OPI Nail polish question!</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ec4hrn/opi_nail_polish_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1ec4bc8</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>What is the most distracting polish you own? Can be blinding or distractingly beautiful</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ec4bc8/what_is_the_most_distracting_polish_you_own_can/</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1ec3zp5</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>tried to capture the new holo taco thermal color transition after I washed my hands!</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec3zp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1ec3hf1</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Ok ok, I get the GLL hype now</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec3hf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1ec37j4</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Blackberries or grapes? 💜</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec37j4</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1ec2zsu</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why is the best lighting always in the bathroom!? First post here, excuse the bad posing. </t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec2zsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1ec2y39</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Decided to try my hand at layering and made this! I love it ! Thoughts? :)</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec2y39</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1ec204s</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Gunmetal, charcoal, and very dark gray or taupe polishes</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ec204s/gunmetal_charcoal_and_very_dark_gray_or_taupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1ec19vr</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Does body chemistry matter, or is it actually the climate?</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ec19vr/does_body_chemistry_matter_or_is_it_actually_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1ec0rce</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>In love with this color after I sliiiiightly customized it  👀</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec0rce</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1ec0hko</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Mooncat, "A Most Destructive Melody" 💜🩵</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3yyek2p7ped1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1ec071y</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Emily de Molly dupe </t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cnc54uq46ped1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1ec05zl</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>ILNP Pixie Party Reminds Me of Ham</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgbq5h9x5ped1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1ebyrw7</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>ILNP Bluebell's sparkle is insane</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4wozbytpvoed1</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1ebyj70</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Maniology top coats: comparing smudge-free vs. aqua topper smudge-free</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ebyj70/maniology_top_coats_comparing_smudgefree_vs_aqua/</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1ebyc3l</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Neon Pineapples</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebyc3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1ebxqny</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Can't capture the glow!</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnqylip3ooed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1ebxmky</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Dupe for Poseidon’s Prize?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qpez9p0anoed1</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1ebx04n</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail kit basics - reccos please </t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ebx04n/nail_kit_basics_reccos_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1ebwweq</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Copper red metallics reccos please!</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ebwweq/copper_red_metallics_reccos_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1ebwsj2</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Love these vibes</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rb2b2xk9hoed1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1ebwio5</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>does anyone know what this filament thing is?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebwio5</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1ebvpsh</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Drive In</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebvpsh</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1ebv16k</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Women Who Knock Rarely Make History- Lyn B</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmrs3z4u3oed1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1ebupah</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>sea glass nails 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebupah</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1ebtx17</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Beachy vibes 🌊</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kjjwpeiuned1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1ebtou8</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Any dupes for the warm state of Deeply Superficial from Holo Taco? It's the perfect pink nude I've been searching for, so a non thermal version of this is a must! Ft. Sugar Rush (Holo Taco). Thank you!</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2f34t8hsned1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1ebpvm8</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Accidentally matched my pyjamas. I’m not lying. 🤷‍♀️💜</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbye9t3ummed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1echc4c</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Summer vibes with blooming gel 🧡🩷</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ploulic36ted1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1ecg5an</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Strawberry Nails 🍓</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecg5an</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1ecf8lb</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>😍</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nx6ze3mzised1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1ecea3r</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>recent press ons I’ve made ❤️</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecea3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1ecdm9o</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thank you for helping me find this 🔮 </t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/am88flt63sed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1ecb3qc</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Diy sprinkle nails!</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecb3qc</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1ecaizd</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Strawberry Nails </t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cc6k2ulbred1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1ecagn8</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Olive nails 🫒🫒</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecagn8</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1ec7lby</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Simple and delicate</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec7lby</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1ec7gxe</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>i love my square nails🎀</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec7gxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1ec69h5</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Do airbrush machines for nail smoke up?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ec69h5/do_airbrush_machines_for_nail_smoke_up/</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1ec2s5l</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Love</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5j7pgnsoped1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1ec00l7</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Anime Nails 💖</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ec00l7</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1ebzxl4</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails i did ❤️🫧 </t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ebzxl4</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1ebz3zf</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>delicate and simple with a touch of tenderness💅😍</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7xg6f87yoed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1ebxbtm</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Air bubbles and charm difficulties</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejs288b3loed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1ebu2ip</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Afro Samurai Nails 😍</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qczvgwqsvned1</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1ebts1n</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer nails </t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2phx7y9tned1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1ebsm57</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Cheers 😂</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0urz6k9ined1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jul 27 08:08:06 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_28.xlsx
+++ b/data/2024_07_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C978"/>
+  <dimension ref="A1:C1135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17059,6 +17059,2675 @@
         </is>
       </c>
     </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1edaeiv</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>11th set</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edaeiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1eda2el</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>10th set</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eda2el</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1ed6td9</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Any tips for picking nail polish off with less damage to the nail?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ed6td9/any_tips_for_picking_nail_polish_off_with_less/</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1ed7rwa</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ombre style nail art tips? </t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ed7rwa/ombre_style_nail_art_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1ed7jgd</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! Press on nails question </t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inn62plnkzed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1ed6gxh</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recovering from acrylics </t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ed6gxh/recovering_from_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1ed6dfg</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>🤩</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/243b7gzz8zed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1ed5trp</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set I've done since Oct. 2021. How do the shorties suit me? </t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed5trp</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1ed5tt7</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>What’s worse? Dip or press-ons?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ed5tt7/whats_worse_dip_or_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1ed5pog</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>She was a fairy</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed5pog</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1ed5a8j</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t xml:space="preserve">😫😫😫 I hate it when this happens </t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bf54i8bgyyed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1ed0cw7</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Husband finds my inspo</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed0cw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1ed21tf</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Just got my first gel set and I’m not understanding the safety of it.</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ed21tf/just_got_my_first_gel_set_and_im_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1ed2lum</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>My first DIY acrylic set</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed2lum</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1ed2ofd</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Nail Polish help</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/klsq4f43byed1</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1ed3p4k</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Nail damage</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kiygtgkvjyed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1ed4lxy</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Clip-on nails?</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ed4lxy/clipon_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1ed4crz</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Show Me Y’all’s Coolest Nail Set(s)!</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed4crz</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1ed37b9</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>My mom is my nail tech</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2p71q8uhfyed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1ed33wh</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>People who use gel nail polish</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ed33wh/people_who_use_gel_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1ed33jt</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Baby Shower Nails</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6z1er2bleyed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1ed2sxa</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>My favorite thing to add to nails for the past 5 years.</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u058tgh4cyed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1ed2hei</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing press ons </t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70vqu29f9yed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1ed22ns</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Red!!! ❤️</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6q5b3xjy5yed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1ed1xed</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>"Enchanted forest" was the request</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed1xed</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1ed1vft</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Summer nails - first time trying a different color on two nails and I love it!</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed1vft</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1ed1ifr</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>New Pressons for my self</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed1ifr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1ed14t0</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>freestyle set</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed14t0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1ed0p8s</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>9th set Comicon Y'all!</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/un70xbbuuxed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1ed0kjc</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Aura nails want vs. got</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxs15p1stxed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1ed07cm</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>painted these for a festival :)</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed07cm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1ed06gv</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed06gv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1ed00zg</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>My boyfriend lets me practice doing nails on him 💅</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed00zg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1eczuvl</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Nail Tech Killed This Set </t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eczuvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1ecz2cv</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>First full set of press ons! 18f</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3xhgxn2ixed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1ecy0d2</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Need help looking for, long round pastel pink nails with pink French tips and whatever else design</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ecy0d2/need_help_looking_for_long_round_pastel_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1ecyk2g</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Simple, shimmery pink 🌸</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecyk2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1ecy7kp</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Throw the whole hand away</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zkuiip1kbxed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1ecxx19</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>How can I prevent DIY gel nails from peeling/chipping after only a few days?</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/luk6kjw89xed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1ecxugo</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>press on set I made! Loving the colors 🌈</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ysumf1gp8xed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1ecx0yo</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Why do I get these marks later on after doing my gel nails?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rcxz1psg2xed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1ecwpha</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>I love them in white</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smrvn5j00xed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1ecw006</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>The sea on my nails and in my soul 🤍🩵💙</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecw006</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1ecvmi2</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Obsessed with the latest designs my nail artist did on me ✨</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecvmi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1ecuuio</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Where to get DND Gel in Canada?</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ecuuio/where_to_get_dnd_gel_in_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1ecuis9</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Aqua chrome</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45h1y5qejwed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1ecubpo</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Friends daughter made my nails</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecubpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1ecu8cu</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Absolutely LOVE my new set 😍</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/911alh38hwed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1ecu4lt</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Meet Alex - New set ‘Punk’ part VIII</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rigqzs0hgwed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1ectwtp</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>New summer nails 🦚</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ectwtp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1ectrs2</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>In need of Player 2, who's gonna join?</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkubaj4tdwed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1ectg44</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Can someone help me fix my nails</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ectg44</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1ecss7v</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Made myself some pressons and I am obsessed </t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecss7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1ecmfj5</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>So I was thinking...</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hajyvvzysued1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1ecswa6</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Russian Manicure</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecswa6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1ecstvt</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>I got fairy nails again! What do we think? 🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dglrzcdy6wed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1ecsrda</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Iridescent nails</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3jqmpadf6wed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1ecsqca</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best clear coat nail polish for natural nails? </t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecsqca</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1ecsi5w</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Easier methods for the ridges</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ecsi5w/easier_methods_for_the_ridges/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1ecsffz</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Sharing my favorite soft gel set. Felt cute and coquette with this one. 🎀</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iswupnoy3wed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1ecsdbm</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tapered coffin... Thoughts? </t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecsdbm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1ecrtm0</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Emerald loveeee 💚💚💚</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecrtm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1ecrnse</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Clean and simple 🩷</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cccqbat9yved1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1ecqv23</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Cute Japanese Theme</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecqv23</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1ecqe62</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Every girl needs glitter in their life ✨️ </t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y52gvjs1pved1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1ecqau3</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Some of my favorite seasonal nails (at home attempts)</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecqau3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1ecpk4j</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Finished in an hour</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n20rzx7yived1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1ecpjy4</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Natural nails with Catrice base coat</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xub4s8uwived1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1ecpfl3</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>The cutest set</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thjzkxszhved1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1ecpa4x</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Neon and Gold for brat summer 💛🌟👑🤗</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/niimhddugved1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1ecou3o</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>OMG Kiss Acrylics are Fantastic</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecou3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1ecosvo</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Blooming Gel</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecosvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1ecnp13</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Feeling creative!</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecnp13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1ecmvd6</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wanted to try the new nude but had to jazz it up. </t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecmvd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1eclaxq</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Pool party💙</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdt3t6muhued1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1eckc4k</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>press-on nailsets that I made on the early July</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eckc4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1eck88m</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Accidentally broke my nail on index finger so had to trim it out. Should I cut down others too?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdsusx0o5ued1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1ecjrt4</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Counting down to Halloween</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/am3po8q00ued1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1eciuja</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Light stain where fingertip meets the nail</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eciuja</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1edayf1</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Best black &amp; red nail polish shipping to Singapore?</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1edayf1/best_black_red_nail_polish_shipping_to_singapore/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1edaao1</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does lighter polish cause yellow stained nails? </t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1edaao1/does_lighter_polish_cause_yellow_stained_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1ed7afx</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>3 month nail growth! thank you all!</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed7afx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1ed73yq</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Umm???? Has anybody else had this issue with Mooncat's matte polish formula? It won't seem to cure properly, even though I did my standard procedure. Never had an issue like this before with Mooncat, or any other brand's matte polish...it's like, fudgy.</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed73yq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1ed71mw</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>PSA: Major Staining</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed71mw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1ed70ue</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Light Laquear French nail brush </t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ed70ue/light_laquear_french_nail_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1ed6z9y</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>What is the grossest polish you can think of?</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ed6z9y/what_is_the_grossest_polish_you_can_think_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1ed6xo6</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Do you like reds? Do you like 'em BRIGHT?</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed6xo6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1ed6tp8</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>For decanting Mooncat polishes, I recommend Indigo Bananas. Bonus: the original brushes fit!!</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vnwmarddzed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1ed6im0</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>It's not just Mooncat it seems.....</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed4c7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1ed698l</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>For those that do nail art with regular polish/lacquer, what brushes are you using?</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ed698l/for_those_that_do_nail_art_with_regular/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1ed65ml</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Hozier Nails!</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed5y9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1ed613s</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer You, of Unshakable Conviction</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed613s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1ed5hgc</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>I got Cygnus Loop in the mail today 🙌🏻🙌🏻</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jy9k47cd0zed1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1ed5etq</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>In celebration of the Olympics / Pour célébrer les jeux Olympiques à Paris</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trmrjgfozyed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1ed4heh</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Which base coat do you apply first before Orly base coat to prevent damage?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ed4heh/which_base_coat_do_you_apply_first_before_orly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1ed44v2</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Bees Knees, Elden Beast + Mooncat, Fools Gold Topper ✨</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpisoemknyed1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1ed3j5h</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>glass jellyfish by lumen 🪼</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qqfsfnciyed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1ed2zro</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Emerald shards is dead</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfuf0qyodyed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1ed2yph</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>First time trying nail art!</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed2yph</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1ed2yk2</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>what do i need to know to safely make press on nails like this at home?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed2yk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1ed2gu9</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Sale Alert: LynB &amp; Death Valley Nails!</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ed2gu9/sale_alert_lynb_death_valley_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1ed252k</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you prefer a thick gel-like thickness to a manicure or a thinner look? Has your opinion changed? </t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ed252k/do_you_prefer_a_thick_gellike_thickness_to_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1ed1phe</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Why yes I have been salivating waiting for the Lurid Lacquer drop how did you know?</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bloorrgx2yed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1ed1bo0</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! Top of nails keep peeling and I have no idea why. I never use harsh chemicals use them while wet and use nail polish sparingly, never gel. I try to repair the nail with a clear tip coat, but it still peels. I usually have to clip them when they get bad and it's so annoying :( any idea why? </t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed1bo0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1ed15jl</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>🧱the rust that grew between telephones🧱</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f906jnfgyxed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1ed0r2y</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Man I just love “Oh Splat!”</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed0r2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1ed03aj</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Olympic athlete nail art </t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ed03aj/olympic_athlete_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1ecz5pq</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Probably a terrible idea….</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ecz5pq/probably_a_terrible_idea/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1ecyo9d</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Deadpool &amp; Wolverine nails 🩸⚠️</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecyo9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1ecyltl</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Geometric Waves ft. My dog who wouldn’t stop trying to hold my hand.</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecyltl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1ecyk16</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Narf Atomic Polish</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4n4xve9exed1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1ecxwrp</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lumen I Axolotl Questions </t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecxwrp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1ecxssc</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Need help looking for, long round pastel pink nails with pink French tips and whatever else design</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ecxssc/need_help_looking_for_long_round_pastel_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1ecx64h</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>ORLY Fall 2024 - Terra Nova (Color Pass Review)</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecx64h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1ecwpg4</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First post! Deadpool inspired nails </t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecwpg4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1ecwlzb</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>How often does Hypnotic Polish restock their out of stock items?</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ecwlzb/how_often_does_hypnotic_polish_restock_their_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1ecwkzq</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Best Clear Nail Stamper?</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ecwkzq/best_clear_nail_stamper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1ecwhoe</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mani roundup for July! </t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecwhoe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1ecw5ry</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>For people in the EU, where do you order American polish brands without having to spend a fortune on shipping costs?</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ecw5ry/for_people_in_the_eu_where_do_you_order_american/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1ecvlxq</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Zoya haul</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qctxj8krwed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1ecvdmb</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Sunshine on the nails, NOT on the application</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yftohuftpwed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1ecvc3x</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Holo Taco holos make really good gradients</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecvc3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1ecuihb</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecuihb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1ectuuq</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Dig this groove- Great Lakes lacquer</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ri93psfewed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1ectgzy</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>July manis! Death Valley Nails, Cirque, and Cracked Polish Swatches</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ectgzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1ectb74</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Moving soon… what to do with my collection?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ectb74/moving_soon_what_to_do_with_my_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1ect630</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Polish getting thick quickly while applying it?</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ect630/polish_getting_thick_quickly_while_applying_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1ecrs73</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Citrusy Jelly Skittle 🍋‍🟩✨</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecrs73</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1ecqt0k</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Grimoire glitz - Cirque colors</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecqt0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1ecqay6</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Help! I want to recreate this look with non-gel polish. Any recs?</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1fcf43goved1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1ecq6zc</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>I don't need to file every time I do press ons?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ecq6zc/i_dont_need_to_file_every_time_i_do_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1ecp4ub</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Seche Vite / Mooncat Brush?</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ecp4ub/seche_vite_mooncat_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1ecp2ky</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Flower Child for warm-toned/olive PoC?</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ecp2ky/flower_child_for_warmtonedolive_poc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1ecog4a</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>First attempt applying gel polish💫</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4rp730jfaved1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1ecnwk1</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>LynB does these glowy polishes soooo well</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c76c59xz5ved1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1ecnv0p</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Glampire 🦇</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ehjjwu3a5ved1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1ecmbk2</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>ILNP - showstopper 🍇</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsj69v80sued1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1eclxrm</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does someone have swatches of both HT sacrificial lacquer and ILNP poison? Which do you prefer? </t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eclxrm/does_someone_have_swatches_of_both_ht_sacrificial/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1ecl6n9</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Laying base coats?</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ecl6n9/laying_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1eck4yz</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>cirque colors chemistry or kbshimmer love at frost sight - silver magnetic topper</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eck4yz/cirque_colors_chemistry_or_kbshimmer_love_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1edb1ha</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Holo Stamping</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fnj539zoo0fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1edarga</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>How far I've come in three weeks! (Still haven't painted a real nail yet though)</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rvvapjk2l0fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1ed8j20</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Cat on moon 🐈‍⬛🌖</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqje66lyuzed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1ed7rba</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail polish blending ideas? </t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ed7rba/nail_polish_blending_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1ed7mcn</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>rebuilding these princess nails 💘💅</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed7mcn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1ed5ldi</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Nails I painted for my divorce hearing 💅🏼💚</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed5ldi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1ed3quz</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>subtle ✨️</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3l0iivwakyed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1ed331r</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Baby Shower Nails </t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dgu89jvgeyed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1ed1ypo</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>'Enchanted Forest" was the request</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed1ypo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1ed0ztx</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Story telling nail art, click to view the story of the Duke Bunny </t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ed0ztx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1ed0ak4</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>mixing three colors  is the new normal.</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/woi7ogqkrxed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1ecw1y4</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>The sea on my nails and in my soul 🤍🩵💙</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecw1y4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1ecspbi</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Started to make myself some pressons for ease - I actually love them way more than I thought I would </t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecspbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1ecsbjp</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Pilachu nails!</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e03efip53wed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1ecob8y</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Googly eye!</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecob8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1ecnkwe</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Experimental set for my videographer!</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ecnkwe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1eclwhs</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Newbie (about a week)</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99w4ehtxnued1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jul 28 08:08:05 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_28.xlsx
+++ b/data/2024_07_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1135"/>
+  <dimension ref="A1:C1315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19728,6 +19728,3066 @@
         </is>
       </c>
     </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1ee1xei</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>My first time using BIAB - how can I improve?</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ee1xei</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1ee06i9</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Summer Olympic Nails</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fmz5yy047fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1edzyeu</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>How to use press-on nails?</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edzyeu/how_to_use_presson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1edz2d0</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Why does my top coat do this?</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygc477for6fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1edy3v2</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Bug spray made my pedicure matte</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edy3v2/bug_spray_made_my_pedicure_matte/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1edy3p4</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail business </t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edy3p4/nail_business/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1edxduo</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Where can I find fake nails of only 0 size?</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edxduo/where_can_i_find_fake_nails_of_only_0_size/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1edx3om</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>gouged my nail 3 years ago and it still looks like this :(</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axof5ngg76fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1edvtlq</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Do I demand a refund? Inspo found on Pinterest from @ashtravv</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edvtlq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1ee0mmk</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Summer Vibes!!!!</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ee0mmk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1ee0lz7</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">just got into nails! here’s my first set of every day / day time / grocery store nails </t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kr3awf397fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1ee027u</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>First time getting nails done</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ee027u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1edz8nu</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>gel x over my natural nails</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjsk8selt6fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1edy97m</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>My new set</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qwhagk9j6fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1edy71l</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Simple designs</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edy71l/simple_designs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1edxnrw</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>These press ons!</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2htogqe2d6fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1edxkdd</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>my new set 🍒🎀</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edxkdd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1edxk4n</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>My latest mani 🩵</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/arcfnvk2c6fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1edx3it</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Love a good bright mani</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edx3it</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1edwxtj</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got these lime nails, and they’re making me so stinking happy </t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxd55zwt56fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1edwrrl</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>New Gel-X set I did</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfb4jzk646fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1edwroq</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh Gel-x set featuring new tattoos </t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hg59m8c546fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1edwr5c</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>First attempt at aura nails</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/miszh9j046fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1edwpqu</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Nice and simple 🤍✨</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ndvn1e8m36fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1edwlvq</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>My first gel-x set on someone else!</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edwlvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1edwko9</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A little uppdate post with more picks for those who dont believe that it is my boyfriends nails </t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edwko9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1edtjxk</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Inspo vs Result 🩵</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edtjxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1edsopa</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Feeling defeated… about to give up</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edsopa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1edvmjt</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Here is my new set of Nezuko Kamado’s nails from the anime, Demon Slayer 🥹</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tg7wm9s1t5fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1edvhf7</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>I love how I didn't have any ideas for my nails appointment so I choose a color and my nails artist just did something she wanted :)</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxx1hjkpr5fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1edve85</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just finished these and love them </t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10p5jynuq5fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1eduhyf</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>First time using ohora nails</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eduhyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1edu7r1</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Cute little gel set</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ve8kvlzwf5fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1edtz1p</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>I'm working on my first ever set with gel polish. Any ideas how I could do the thumb?</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnhn2nqtd5fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1edtuki</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>My 1st and 2nd time trying nail art</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edtuki</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1edtqle</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How bad are they? </t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edtqle</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1edthkb</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kinda pleased with these press ons I made for myself! </t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edthkb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1edtcia</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need help figuring out what type of product I want to get a full set of. </t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edtcia/need_help_figuring_out_what_type_of_product_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1edtc2q</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edtc2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1edt0q6</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>My nail tech 🫡</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1qpe1ur55fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1edsgoq</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Set I did on my friend c: ✨</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edsgoq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1edrxky</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>I got my nails done for the first time. Am I wrong for being a little upset ?</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edrxky</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1edri1k</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Butterfly nailart 🦋</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/37hslrv3t4fd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1edrett</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>New set!! I usually get pink but decided to go white for the end if summer</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aunujpsfs4fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1edrdiw</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Anyone here bakes regularly?</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edrdiw/anyone_here_bakes_regularly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1edr870</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Should I ask to have them redone?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94k23i6xq4fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1edqt9i</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Cracked gel nails</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edqt9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1edqqgl</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>One week later. Still obsessed!</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edqqgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1edqpwy</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Fake nail brands?</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edqpwy/fake_nail_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1edqmeu</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Another stunning abstract builder gel manicure from my nail tech!</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jab1g99zl4fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1edqi0h</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Aluminum foil vibez 🩶</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ynufsh1l4fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1edo2cr</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Nail tech didn’t take off all of my acrylics??</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfaqo1hw14fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1edod5b</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>I think I made a masterpiece 🥹 how do you rate them?</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edod5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1edoe9x</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>First time doing nails for unfamiliar client</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edoe9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1edp6us</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Did I do a good job with my cuticle?</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edp6us</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1edpvti</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>I wanted my nails to match my dress</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/svx4fvg4g4fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1edpu29</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>(women only) nail color and shape research survey !!</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edpu29/women_only_nail_color_and_shape_research_survey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1edpo6w</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>super weak nails</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edpo6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1edpa8k</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Nails (M)</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwrcx58fb4fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1edp9t8</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>I work at a fragrance store and the alcohol messes up my nails. Any solution?</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edp9t8/i_work_at_a_fragrance_store_and_the_alcohol/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1edp8ft</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The girl doing my pedi had the cuuuutest nails I’ve ever seen (she gave me permission to post)  </t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a48ih4l8b4fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1edp033</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I become a nail tech without having to do nail art? </t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edp033/can_i_become_a_nail_tech_without_having_to_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1edom26</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>In love with my new nails. First time I've done multicolor and 3D</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edom26</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1edom0s</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Loving this new set!</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5srwfiw964fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1edof3a</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t xml:space="preserve">POWERPUFF GIRL BUTTERCUP NAIL ART TUTORIAL </t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://vm.tiktok.com/ZGeWQw3CS/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1edo8t9</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder gel issues </t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edo8t9/builder_gel_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1edo6gm</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Warehouse Nails</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edo6gm/warehouse_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1ednbgd</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I overreacting? Or are these okay? </t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ednbgd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1ednt70</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Floral gel manicure</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ednt70</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1ednff3</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Attempt #1: My Builder Gel Mani looks horrible. Any advice is appreciated. </t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ednff3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1edne7o</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>First attempt using gel nail polish💫</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6y3vl6imw3fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1edn5qp</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Too short for almond?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edn5qp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1edn09w</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>peach trees 🍑🍃</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edn09w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1edmxdp</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Does normal nail polish last longer from than salon vs doing it yourself?</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edmxdp/does_normal_nail_polish_last_longer_from_than/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1edmb31</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Should I be upset about the cuts on my cuticles?</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edmb31</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1edbjnl</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Extremely frail nails after acrylics</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edbjnl/extremely_frail_nails_after_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1edg8jo</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>How can I make it better?</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edg8jo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1edjvkt</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Manicure with gel color and gel builder</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xiu511q153fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1edmnao</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Lifting along cuticle</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/67r1d8ltq3fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1edmkc5</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>My new set</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q345q1g6q3fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1edmdzw</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>My nails matched my drink! (Excuse my awkward poses. Lol)</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edmdzw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1edm6bj</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Split toe nail</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edm6bj/split_toe_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1edm5jr</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Do almond nails suit me better than tapered square?</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edm5jr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1edm3o1</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gave my husband about 20 wrap choices and told him to pick one for fun. After careful consideration he chose this. </t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edm3o1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1edm129</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Summer nails 🩵</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/da5wvhqzl3fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1edlx4m</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Glam Goth Nails</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edlx4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1edlvih</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Love this color!!!</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3jwcrojpk3fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1edlu9z</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wider press ons? </t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edlu9z/wider_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1edlg4u</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">builder gel vs russian manicure nyc recommendations </t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edlg4u/builder_gel_vs_russian_manicure_nyc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1edleet</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/234e2u6zg3fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1edl6rk</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>🌸💛</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edl6rk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1edl4xa</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>first nails I've ever done myself without getting a chip in 5</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inqal4bxe3fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1edl19g</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>A long time overdue</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0n36apq6e3fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1edkxbc</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Youtube tutorial for leveling polygel with e-file</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1edkxbc/youtube_tutorial_for_leveling_polygel_with_efile/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1edkkkh</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Textured nails</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edkkkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1edkjpq</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>solid classic :)</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7z2eh0n9a3fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1edkac5</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>I love the new set I just gave myself.</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edkac5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1edk96j</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Peachy keen 🍑</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jq1ce91083fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1edk731</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>just want to show them off 🧡</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edk731</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1ed53rv</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Can someone help me find these? I cant find the brand or anything else except one seller on amazon, its almost like it doesnt exist, its weird. These were the perfect length, shape, and flexibility while still beign durable for my lifestyle. Im out but cant find them anywhere, please help!!</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nbguahxiwyed1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1ee1a7v</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer Lorraine.</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ee1a7v/ethereal_lacquer_lorraine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1edsive</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Tips for getting press ons to stay on?</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zwv0huj15fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1edznrr</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>A more purple/blue version of glass frog</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edznrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1edyakm</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Toppers over white creme</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/bpn4T03</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1edx035</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>This is one of my top 5 manicures of this year🤗</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edx035</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1edwb7g</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>I used gel polish to touch up badly scratched rims</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edw5wq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1edv42s</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Sunshine on my nails ☀️</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edv42s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1edudh0</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favorite ILNP Polishes? </t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1edudh0/favorite_ilnp_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1edu4va</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Wanted to do a muted green for my next mani - help me choose?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icpaw5j7f5fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1edu470</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Placed my first Lyn B order 💅</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fouibq1f5fd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1edtcsu</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Desperately needed a palette cleanser … and I’m obsessed 🔥</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edtcsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1edsy3y</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First-time Gel X application </t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edsy3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1edsvja</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Ladies and gentlemen, ✨her✨</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edsvja</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1edscam</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Essie Special Effects</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1edscam/essie_special_effects/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1edsars</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Dark red jelly nail polish?</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nopml80mz4fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1edqub1</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>First color4nails purchase ☺️</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kf7jwasn4fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1edqpjh</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Cirque Colors swatches</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edqpjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1edqfd6</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Mentally rebranding Pumpkin Patch to "Sunshine" for the summer</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68oq6ebgk4fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1edq7re</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A glittery experiment </t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edq7re</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1edpnjy</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>I layered some pink flakies over House of Hades</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5hhcgkge4fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1edp34f</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Are we down for darker shades in the summer?</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rv2len94a4fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1edp02o</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Deeply superficial 🍓</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edp02o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1edoujx</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>BKL Get Lobstered vs Ethereal Ether Dragon</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0clo32f684fd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1edot9z</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>In love with this color combo</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edot9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1edocdm</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Lush</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edocdm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1edo36p</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Sorting my greens and blues makes me question my sanity and my life choices</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edo36p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1ednn9x</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer You Are the Rock That Refuses</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ednn9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1edmvpb</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>So hard to capture this one! - Belladonna by Monarch, PPU Rewind July 2024</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edmvpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1edmjhx</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Cirque Colors Kokomo 🩵</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x27vgb00q3fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1edmeoo</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>My first LynB haul is a doozy</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edmeoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1edme4u</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Purple Slushie by Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdouoqkxo3fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1edlnhi</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Did I just ruin my OPI polish?</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/febsvi7zi3fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1edlrc9</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>RL Discord Moderating Issues</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1edlrc9/rl_discord_moderating_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1edllcb</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Mysterious Uranus</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edllcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1edldgn</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Some DVN swatches 😊</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1ll2epoqg3fd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1edl72x</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Usually a dark red girl, decided to go for a new look</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edl72x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1edkonj</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>So in love with subtle glitter</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1rzqgleb3fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1edkl5k</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glisten and glow top coat has changed my life </t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edkl5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1edkcdx</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Layla Rarity Beo </t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edkcdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1edkbxy</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>BKL Get Lobstered</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzr7svzl83fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1edk7zd</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>the way i almost skipped out on Flower Child 😭</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edk7zd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1edjz8x</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Happy brat summer to all who celebrate 💚</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edjz8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1edjybu</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP - Poison </t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lj985tii53fd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1edjwny</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>A flowery one today</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfyqc8ya53fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1edjfav</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>ILNP Sale?</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1edjfav/ilnp_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1edj1cs</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bee’s Knees Lacquer FFS </t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edj1cs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1edj0om</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Abomination Polish - Cinderella</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0vxjnfnx2fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1edi91m</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Order fulfillment? </t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1edi91m/order_fulfillment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1edhid6</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Opinions on OPI Infinite Shine Base Coat? Does it help keep your mani on for long?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1edhid6/opinions_on_opi_infinite_shine_base_coat_does_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1edh3b2</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Pray to whatever the deity for nail polish is, folks! Please?</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1edh3b2/pray_to_whatever_the_deity_for_nail_polish_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1edfooo</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Your best tips for an absolute beginner? (Regular nail polish)</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1edfooo/your_best_tips_for_an_absolute_beginner_regular/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1edegs9</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Did OPI Natural Nail Base Coat cause peeling for you like Orly base coat did?</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1edegs9/did_opi_natural_nail_base_coat_cause_peeling_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1edbvjw</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Bonus track: dead flesh ...purple conditioner for your nails</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7thh9hfz0fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1edbu2b</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Essence top and base coats</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1edbu2b/essence_top_and_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1ee1y29</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Hand painted TØP inspired set i did for a friend</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6msvpydp7fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1ee0t4c</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Perfect mix of vampy vibes and Barbie as Rapunzel 💜</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xr78q4ieb7fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1ee0q62</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>my new fav shape/color combo</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ee0q62</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1ee0kqv</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Not my usual style but I love the end result!</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ee0kqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1ee05zh</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t xml:space="preserve">summer vibes </t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/stzatrhu37fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1ee006f</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Perfect for w wedding right!?! </t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3h1066ix17fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1edxgeu</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Are there press ons to remove before work and apply back on afterwards?</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1edxgeu/are_there_press_ons_to_remove_before_work_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1edxdbv</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>I really love my almond design🩶</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edxdbv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1edwzxz</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/boftbv6f66fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1edvwbg</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed with this month’s set! My girl killed it. </t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edvwbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1edvqjk</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Summer flowers</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edvqjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1edugyf</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Five months into learning to do my nails at-home and I'm starting to like what I see 🥰</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edugyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1edrfwt</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Butterfly Nailart made by me🦋</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6uqyaq6os4fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1edr0wl</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>What yall think?</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edr0wl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1edq5s4</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>my current nails</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z76ulgrci4fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1edpmoj</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Practicing with colours and blooming gel</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edpmoj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1edoegc</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BUTTERCUP FROM POWERPUFF GIRL TUTORIAL </t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://vm.tiktok.com/ZGeWQw3CS/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1edncbv</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Starry Nails ⭐️ </t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7p01muw7w3fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1edmy4a</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>✨🎀Y2K hello kitty🎀✨</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fyjj944t3fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1edmlua</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Textured Nails</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edmlua</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1edkojn</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>I did my nails for an event tonight.</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1gw55vdb3fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1edi8at</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Custom set for Alexandra 🪲</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edi8at</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1edhkyr</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>First Set On Someone Else</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bahcrgkqm2fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1edgona</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Need more practice. :)))</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9ldn9m2f2fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1edbsnl</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Some of my faves from recently</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1edbsnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1edbrxe</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Polygel set</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lwybov1y0fd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>